<commit_message>
codigo para fazer os teste sem instruções ainda
</commit_message>
<xml_diff>
--- a/Aula14/tabelinha.xlsx
+++ b/Aula14/tabelinha.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesComp\DesignComp-Projeto2\Aula14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143B5EB6-91E2-465D-8A55-B9EF860F3938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2874A038-8008-4C7F-AEDC-E474B4AFFE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{B56DCD25-DD30-4F59-AF24-F1D9751F2CAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{B56DCD25-DD30-4F59-AF24-F1D9751F2CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>LW</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Escreve</t>
+  </si>
+  <si>
+    <t>MUX ULA mem</t>
+  </si>
+  <si>
+    <t>MUX Rt/Imediado</t>
+  </si>
+  <si>
+    <t>MUX Rt/Rd</t>
   </si>
 </sst>
 </file>
@@ -451,24 +460,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E197772-8A56-4E87-AD77-079DF697BC4B}">
-  <dimension ref="C2:J13"/>
+  <dimension ref="C2:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
@@ -479,22 +491,31 @@
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -505,7 +526,7 @@
         <v>100011</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -517,10 +538,19 @@
         <v>1</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -534,19 +564,28 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
@@ -560,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -568,54 +607,71 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -624,6 +680,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="286ddd33-a286-4f05-bbf4-221dca8b255d">
@@ -635,15 +700,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -850,19 +906,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{763A0F2F-7799-4727-AA2D-7D98108F00E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A789EBDB-4E62-475A-A513-8515145C5351}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="286ddd33-a286-4f05-bbf4-221dca8b255d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{763A0F2F-7799-4727-AA2D-7D98108F00E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>